<commit_message>
~ changes in ccfgs files and create_fixed now requires .xlsx
</commit_message>
<xml_diff>
--- a/examples/oucru/oucru-01nva/resources/outputs/templates/ccfgs_01nva_data_fixed.xlsx
+++ b/examples/oucru/oucru-01nva/resources/outputs/templates/ccfgs_01nva_data_fixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelda\Desktop\repositories\github\datablend\main\examples\oucru\oucru-01nva\resources\outputs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DCADF8-D83A-40D0-8C46-352FE4CCCA8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D0D37F-CAD1-45AB-9EED-4B3C1BAF4AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27195" yWindow="1080" windowWidth="23730" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28455" yWindow="3195" windowWidth="47250" windowHeight="9900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DM" sheetId="1" r:id="rId1"/>
@@ -1788,9 +1788,6 @@
     <t>conscious_description</t>
   </si>
   <si>
-    <t>ventilation</t>
-  </si>
-  <si>
     <t>{3: 3}</t>
   </si>
   <si>
@@ -1819,6 +1816,9 @@
   </si>
   <si>
     <t>occupation</t>
+  </si>
+  <si>
+    <t>ventilation_type</t>
   </si>
 </sst>
 </file>
@@ -2277,7 +2277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2376,7 +2376,7 @@
         <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -2393,7 +2393,7 @@
         <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -2469,7 +2469,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C10" t="s">
         <v>85</v>
@@ -4438,8 +4438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4883,7 +4883,7 @@
         <v>263</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>578</v>
+        <v>588</v>
       </c>
       <c r="C24" t="s">
         <v>84</v>
@@ -6152,7 +6152,7 @@
         <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -6169,7 +6169,7 @@
         <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -6236,7 +6236,7 @@
         <v>97</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>86</v>
@@ -6516,7 +6516,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -6904,7 +6904,7 @@
         <v>133</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>84</v>
@@ -6955,10 +6955,10 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C50" t="s">
         <v>88</v>
@@ -6969,10 +6969,10 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C51" t="s">
         <v>88</v>
@@ -6995,10 +6995,10 @@
         <v>1</v>
       </c>
       <c r="G52" t="s">
+        <v>581</v>
+      </c>
+      <c r="H52" t="s">
         <v>582</v>
-      </c>
-      <c r="H52" t="s">
-        <v>583</v>
       </c>
       <c r="I52" t="s">
         <v>402</v>
@@ -7087,7 +7087,7 @@
         <v>571</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L56" t="s">
         <v>401</v>
@@ -10277,7 +10277,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -10420,8 +10420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>